<commit_message>
keys inside config, written DAG
</commit_message>
<xml_diff>
--- a/matchweek_date_mapping.xlsx
+++ b/matchweek_date_mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04e22f51a73b2b94/Documents/football_analytics_git/football_analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F24B5476-3391-4E8C-808C-03076FE56E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{F24B5476-3391-4E8C-808C-03076FE56E75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30DAB904-5D3C-49AB-AD63-F962A43714D8}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{F6AFF93F-F61A-47A9-86A2-50853B585453}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F6AFF93F-F61A-47A9-86A2-50853B585453}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -57,10 +57,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF3B3B3B"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <sz val="11"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -421,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DEC14A-1B88-499C-9115-EBD32904687A}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -433,7 +433,7 @@
     <col min="2" max="2" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -449,7 +449,7 @@
         <v>45513</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -459,7 +459,7 @@
         <v>45520</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A14" si="0">A3+1</f>
         <v>3</v>
@@ -469,7 +469,7 @@
         <v>45527</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -478,8 +478,9 @@
         <f t="shared" ref="B5:B14" si="1">B4+7</f>
         <v>45534</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -489,7 +490,7 @@
         <v>45541</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -499,7 +500,7 @@
         <v>45548</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -509,7 +510,7 @@
         <v>45555</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -519,7 +520,7 @@
         <v>45562</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -529,7 +530,7 @@
         <v>45569</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -539,7 +540,7 @@
         <v>45576</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -549,7 +550,7 @@
         <v>45583</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -559,7 +560,7 @@
         <v>45590</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>

</xml_diff>